<commit_message>
v4: flow and specs added
</commit_message>
<xml_diff>
--- a/v4/documentation/Specs_v4.xlsx
+++ b/v4/documentation/Specs_v4.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victoriadudley\Desktop\Team-Infinite\v4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew.bulley\Team-Infinite\v4\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>If both distances are the same, output first ID</t>
   </si>
@@ -132,6 +132,21 @@
   </si>
   <si>
     <t>VERSION4</t>
+  </si>
+  <si>
+    <t>Add exchange button</t>
+  </si>
+  <si>
+    <t>Remove exchange2 row</t>
+  </si>
+  <si>
+    <t>Add dropdown and populate with added exchanges</t>
+  </si>
+  <si>
+    <t>(reset button)</t>
+  </si>
+  <si>
+    <t>(placeholder text)</t>
   </si>
 </sst>
 </file>
@@ -422,7 +437,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
@@ -479,6 +494,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -761,24 +778,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="73.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="73.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="67.44140625" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="67.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -794,7 +811,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="31" t="s">
@@ -804,7 +821,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -812,7 +829,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="24" t="s">
         <v>18</v>
@@ -828,7 +845,7 @@
       </c>
       <c r="F4" s="26"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="12" t="s">
         <v>32</v>
@@ -838,7 +855,7 @@
       <c r="E5" s="10"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="22" t="s">
         <v>3</v>
@@ -854,7 +871,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="23" t="s">
         <v>5</v>
@@ -870,7 +887,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="22" t="s">
         <v>2</v>
@@ -886,7 +903,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="23" t="s">
         <v>1</v>
@@ -902,7 +919,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="22" t="s">
         <v>1</v>
@@ -918,7 +935,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="23" t="s">
         <v>4</v>
@@ -934,7 +951,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="22" t="s">
         <v>7</v>
@@ -950,7 +967,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="23" t="s">
         <v>7</v>
@@ -966,7 +983,7 @@
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="13" t="s">
         <v>33</v>
@@ -976,7 +993,7 @@
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="21" t="s">
         <v>16</v>
@@ -992,7 +1009,7 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="21"/>
       <c r="C16" s="9" t="s">
@@ -1002,7 +1019,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="14" t="s">
         <v>19</v>
@@ -1018,7 +1035,7 @@
       </c>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="13" t="s">
         <v>34</v>
@@ -1028,7 +1045,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="21" t="s">
         <v>22</v>
@@ -1046,96 +1063,101 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="36"/>
+      <c r="C20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="37"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="37"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="37"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="37"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="37"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="B25" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="35" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="3"/>
+      <c r="B26" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C26" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D26" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E26" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F26" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="28">
-        <f>SUM(D6:D21)</f>
-        <v>4</v>
-      </c>
-      <c r="E22" s="29">
-        <f>SUM(E6:E21)</f>
-        <v>5.5</v>
-      </c>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="30">
-        <f>SUM(D22+E22)</f>
-        <v>9.5</v>
-      </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="C27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="28">
+        <f>SUM(D6:D26)</f>
+        <v>4</v>
+      </c>
+      <c r="E27" s="29">
+        <f>SUM(E6:E26)</f>
+        <v>5.5</v>
+      </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1143,7 +1165,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1151,15 +1173,20 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="30">
+        <f>SUM(D27+E27)</f>
+        <v>9.5</v>
+      </c>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1167,7 +1194,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1175,7 +1202,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1183,7 +1210,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1191,7 +1218,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1199,7 +1226,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1207,7 +1234,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1215,7 +1242,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1223,7 +1250,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1231,6 +1258,46 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
specs_v4: removed 'display capacity' spec
</commit_message>
<xml_diff>
--- a/v4/documentation/Specs_v4.xlsx
+++ b/v4/documentation/Specs_v4.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>If both distances are the same, output first ID</t>
   </si>
@@ -137,16 +137,10 @@
     <t>Validate capactiy as greater than or equal to 0 and lesser than or equal to 999</t>
   </si>
   <si>
-    <t>Add capacity to exchange display information</t>
-  </si>
-  <si>
     <t>M10.1</t>
   </si>
   <si>
     <t>M10.2</t>
-  </si>
-  <si>
-    <t>M10.3</t>
   </si>
   <si>
     <t>M9.1</t>
@@ -475,7 +469,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
@@ -524,26 +518,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -828,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="41" zoomScaleNormal="41" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1098,7 +1085,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>29</v>
@@ -1116,15 +1103,15 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F20" s="8" t="s">
@@ -1134,7 +1121,7 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>35</v>
@@ -1162,15 +1149,15 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="32" t="s">
         <v>24</v>
       </c>
       <c r="F23" s="8" t="s">
@@ -1179,57 +1166,47 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
-      <c r="B24" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="40" t="s">
+      <c r="B24" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="41" t="s">
+      <c r="D24" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="41" t="s">
+      <c r="E24" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="30" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
-      <c r="B25" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>9</v>
-      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="33">
+        <f>SUM(D6:D23)</f>
+        <v>4</v>
+      </c>
+      <c r="E25" s="34">
+        <f>SUM(E6:E23)</f>
+        <v>5.5</v>
+      </c>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="34">
-        <f>SUM(D6:D23)</f>
-        <v>4</v>
-      </c>
-      <c r="E26" s="35">
-        <f>SUM(E6:E23)</f>
-        <v>5.5</v>
-      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1240,22 +1217,22 @@
     <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="27">
+        <f>SUM(D25+E25)</f>
+        <v>9.5</v>
+      </c>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="27">
-        <f>SUM(D26+E26)</f>
-        <v>9.5</v>
-      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1362,14 +1339,6 @@
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v4: pres and specs update
</commit_message>
<xml_diff>
--- a/v4/documentation/Specs_v4.xlsx
+++ b/v4/documentation/Specs_v4.xlsx
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>